<commit_message>
ajout de la nouvelle version du scrum
</commit_message>
<xml_diff>
--- a/Scruuuuum.xlsx
+++ b/Scruuuuum.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Choses à faire" sheetId="1" r:id="rId1"/>
+    <sheet name="Cas d'usage" sheetId="2" r:id="rId2"/>
+    <sheet name="CRC" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="135">
   <si>
     <t>Faire bouger voiture</t>
   </si>
@@ -225,13 +227,217 @@
   </si>
   <si>
     <t>Maxime</t>
+  </si>
+  <si>
+    <t>ÉVENEMENT</t>
+  </si>
+  <si>
+    <t>VOITURE</t>
+  </si>
+  <si>
+    <t>JOUEUR</t>
+  </si>
+  <si>
+    <t>Fonctions</t>
+  </si>
+  <si>
+    <t>Ordre exécution</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Classe</t>
+  </si>
+  <si>
+    <t>Synthèse</t>
+  </si>
+  <si>
+    <t>AnalyseImage</t>
+  </si>
+  <si>
+    <t>ResultatImage</t>
+  </si>
+  <si>
+    <t>AnalyseVerticale(self)</t>
+  </si>
+  <si>
+    <t>CreerRequete(self)</t>
+  </si>
+  <si>
+    <t>ResultatLaser</t>
+  </si>
+  <si>
+    <t>AnalyseHorizontale(self)</t>
+  </si>
+  <si>
+    <t>self.image</t>
+  </si>
+  <si>
+    <t>def main():</t>
+  </si>
+  <si>
+    <t>def prochaintour(self):</t>
+  </si>
+  <si>
+    <t>def genereAssets(self,participants):</t>
+  </si>
+  <si>
+    <t>def initierSimulation(self,rep):</t>
+  </si>
+  <si>
+    <t>def demarreSimulation(self):</t>
+  </si>
+  <si>
+    <t>def inscritClient(self):</t>
+  </si>
+  <si>
+    <t>self.own</t>
+  </si>
+  <si>
+    <t>self.vue</t>
+  </si>
+  <si>
+    <t>def creeServeur(self):</t>
+  </si>
+  <si>
+    <t>self.modele</t>
+  </si>
+  <si>
+    <t>self.monip</t>
+  </si>
+  <si>
+    <t>def genereNom(self):</t>
+  </si>
+  <si>
+    <t>self.statut</t>
+  </si>
+  <si>
+    <t>self.actions=[]</t>
+  </si>
+  <si>
+    <t>AnalyseLaser</t>
+  </si>
+  <si>
+    <t>def trouveIP(self):</t>
+  </si>
+  <si>
+    <t>self.egoserveur</t>
+  </si>
+  <si>
+    <t>Controleur</t>
+  </si>
+  <si>
+    <t>self.angle</t>
+  </si>
+  <si>
+    <t>self.tempo</t>
+  </si>
+  <si>
+    <t>ComparaisonDistances(self)</t>
+  </si>
+  <si>
+    <t>self.distance</t>
+  </si>
+  <si>
+    <t>def __init__(self):</t>
+  </si>
+  <si>
+    <t>self.cadre</t>
+  </si>
+  <si>
+    <t>Démarrage</t>
+  </si>
+  <si>
+    <t>Joueur pèse sur Démarrer Partie</t>
+  </si>
+  <si>
+    <t>Voiture apparait</t>
+  </si>
+  <si>
+    <t>Scan avec des lasers a 360° (un laser par degrée) pour détecter les obstacles et les voies possibles</t>
+  </si>
+  <si>
+    <t>On stock les résultats de lasers dans une liste de lasers dans AnalyseLaser</t>
+  </si>
+  <si>
+    <t>AnalyseLaser delete le contenu de sa liste</t>
+  </si>
+  <si>
+    <t>Voiture change son angle</t>
+  </si>
+  <si>
+    <t>Voiture commence évenement Avancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Vitesse de voiture augmente</t>
+  </si>
+  <si>
+    <t>Si vitesse de la voiture est inférieure à sa vitesse maximale</t>
+  </si>
+  <si>
+    <t>Voiture fait un scan avec des lasers en 180° en avant d'elle-même (intervalle de 5° par lasers, donc 36 lasers)</t>
+  </si>
+  <si>
+    <t>Lasers enregistrer dans une liste de lasers dans AnalyseLaser</t>
+  </si>
+  <si>
+    <t>AnalyseLaser supprime le contenu de sa liste</t>
+  </si>
+  <si>
+    <t>Si oui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Commencer évènement Tourner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Continuer d'avancer tout droit</t>
+  </si>
+  <si>
+    <t>Répéter chaque 0.2 secondes (Timer dans la classe Voiture)</t>
+  </si>
+  <si>
+    <t>Si non OU si ne détecte pas d'intersection</t>
+  </si>
+  <si>
+    <t>AnalyseLaser envoie la liste à Cerveau</t>
+  </si>
+  <si>
+    <t>Cerveau prends en note les rayons qui détectent un mur à côté de ceux qui n'en détectent pas</t>
+  </si>
+  <si>
+    <t>Cerveau envoie angle où tourner vers -&gt; Modèle -&gt; class Voiture</t>
+  </si>
+  <si>
+    <t>Cerveau calcule angle au milieu de ces rayons et garde en note ce nouvel angle</t>
+  </si>
+  <si>
+    <t>AnalyseLaser envoie sa liste à Cerveau</t>
+  </si>
+  <si>
+    <t>Cerveau utilise donnée pour centrer la voiture (voir Démarrage)</t>
+  </si>
+  <si>
+    <t>Si Cerveau détecte une grande différence entre deux rayons adjacents(detection intersection)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cerveau garde le laser avant la grande différence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cerveau regarde 5 lasers adjacents et garde celle avec des lasers adjacents de plus grande distance qu'elle-même</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Cerveau garde en note l'angle entre les deux lasers</t>
+  </si>
+  <si>
+    <t>Cerveau détermine (RANDOM) si voiture tourne à l'intersection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +451,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,8 +511,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -372,11 +618,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -395,6 +665,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,6 +726,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5291</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123825" y="10344150"/>
+          <a:ext cx="12835466" cy="7219950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -677,7 +1036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -1180,4 +1539,1568 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="119" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:H55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="0.42578125" customWidth="1"/>
+    <col min="4" max="4" width="47" customWidth="1"/>
+    <col min="5" max="5" width="0.42578125" customWidth="1"/>
+    <col min="6" max="6" width="102" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="66.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="37"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G25" s="14"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="14"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G31" s="14"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G32" s="14"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="19"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="5"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="5"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="8"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G55" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="119" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I90"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="21" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="29"/>
+      <c r="B2" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="29"/>
+      <c r="I2" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="28"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="28"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="27"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="35"/>
+      <c r="B5" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="25"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="35"/>
+      <c r="B6" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="35"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="B7" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="25"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="25"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+      <c r="B8" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="26"/>
+      <c r="D9" s="25"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="35"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="25"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="25"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="25"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="35"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="25"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="35"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="25"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="25"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="26">
+        <v>1</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="25"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="25"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="22"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="29"/>
+      <c r="B25" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="34"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="29"/>
+      <c r="I25" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="29"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="34"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26" s="29"/>
+      <c r="I26" s="28"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="25"/>
+      <c r="F27" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="27"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="25"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="35"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="25"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="25"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="25"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="25"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="35"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="25"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="25"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="35"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="25"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="25"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="35"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="25"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="25"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="35"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="25"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="25"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="35"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="25"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="25"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="35"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="25"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="25"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="35"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="25"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="25"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="25"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="25"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="35"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="25"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="25"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="35"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="25"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="25"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="25"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="25"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="25"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="25"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="25"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="25"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="25"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="25"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="22"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="F47" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H47" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I47" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="29"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="28"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="28"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="29"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="28"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="28"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="27"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="25"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="25"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="35"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="25"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="25"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="35"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="25"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="25"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="35"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="25"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="25"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="35"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="25"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="25"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="35"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="25"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="25"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="35"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="25"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="25"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="35"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="25"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="25"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="35"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="25"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="25"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="35"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="25"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="25"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="35"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="25"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="25"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="35"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="25"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="25"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="35"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="25"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="27"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="25"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="25"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="25"/>
+      <c r="F63" s="25"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="25"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="25"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="G64" s="27"/>
+      <c r="H64" s="26"/>
+      <c r="I64" s="25"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="25"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="25"/>
+      <c r="F65" s="25"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="25"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="25"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="25"/>
+      <c r="F66" s="25"/>
+      <c r="G66" s="27"/>
+      <c r="H66" s="26"/>
+      <c r="I66" s="25"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="22"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="22"/>
+      <c r="F67" s="22"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="23"/>
+      <c r="I67" s="22"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D70" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="F70" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="G70" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="H70" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I70" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="29"/>
+      <c r="B71" s="30"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="28"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="30"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="28"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="29"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="28"/>
+      <c r="F72" s="29"/>
+      <c r="G72" s="30"/>
+      <c r="H72" s="29"/>
+      <c r="I72" s="28"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="35"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="25"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="26"/>
+      <c r="I73" s="25"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="35"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="25"/>
+      <c r="F74" s="35"/>
+      <c r="G74" s="27"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="25"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="35"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="25"/>
+      <c r="F75" s="35"/>
+      <c r="G75" s="27"/>
+      <c r="H75" s="26"/>
+      <c r="I75" s="25"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="35"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="25"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="26"/>
+      <c r="I76" s="25"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="35"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="26"/>
+      <c r="D77" s="25"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="27"/>
+      <c r="H77" s="26"/>
+      <c r="I77" s="25"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="35"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="25"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="27"/>
+      <c r="H78" s="26"/>
+      <c r="I78" s="25"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="35"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="25"/>
+      <c r="F79" s="35"/>
+      <c r="G79" s="27"/>
+      <c r="H79" s="26"/>
+      <c r="I79" s="25"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="35"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="25"/>
+      <c r="F80" s="35"/>
+      <c r="G80" s="27"/>
+      <c r="H80" s="26"/>
+      <c r="I80" s="25"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="35"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="25"/>
+      <c r="F81" s="35"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="26"/>
+      <c r="I81" s="25"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="35"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="25"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="27"/>
+      <c r="H82" s="26"/>
+      <c r="I82" s="25"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="35"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="26"/>
+      <c r="D83" s="25"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="26"/>
+      <c r="I83" s="25"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="35"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="26"/>
+      <c r="D84" s="25"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="27"/>
+      <c r="H84" s="26"/>
+      <c r="I84" s="25"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="35"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="26"/>
+      <c r="D85" s="25"/>
+      <c r="F85" s="35"/>
+      <c r="G85" s="27"/>
+      <c r="H85" s="26"/>
+      <c r="I85" s="25"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="25"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="25"/>
+      <c r="F86" s="25"/>
+      <c r="G86" s="27"/>
+      <c r="H86" s="26"/>
+      <c r="I86" s="25"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="25"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="26"/>
+      <c r="D87" s="25"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="27"/>
+      <c r="H87" s="26"/>
+      <c r="I87" s="25"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="25"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="26"/>
+      <c r="D88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="27"/>
+      <c r="H88" s="26"/>
+      <c r="I88" s="25"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="25"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="26"/>
+      <c r="D89" s="25"/>
+      <c r="F89" s="25"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="26"/>
+      <c r="I89" s="25"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="22"/>
+      <c r="B90" s="24"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="22"/>
+      <c r="F90" s="22"/>
+      <c r="G90" s="24"/>
+      <c r="H90" s="23"/>
+      <c r="I90" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A73:A85"/>
+    <mergeCell ref="F73:F85"/>
+    <mergeCell ref="A27:A39"/>
+    <mergeCell ref="A4:A16"/>
+    <mergeCell ref="F4:F16"/>
+    <mergeCell ref="F27:F39"/>
+    <mergeCell ref="A50:A62"/>
+    <mergeCell ref="F50:F62"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="119" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>